<commit_message>
Deploying to gh-pages from  @ ef8601cd20cce18ac4d948b29843af3dcb780e74 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2023_8-1-1.xlsx
+++ b/assets/excel/2023_8-1-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5F1311-BA3A-4A20-A09D-E5297D1F7FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CC0C5E-E04B-441E-8CC8-ADFD73F39A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{1AA46989-31E6-4362-A3EC-DA6643D016B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1AA46989-31E6-4362-A3EC-DA6643D016B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -833,23 +842,23 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:I64"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="42" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="42"/>
+    <col min="1" max="1" width="5.6640625" style="42" customWidth="1"/>
+    <col min="2" max="16384" width="11.44140625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -863,7 +872,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -877,7 +886,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="2:12" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -889,7 +898,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -909,7 +918,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="45"/>
       <c r="C7" s="48"/>
       <c r="D7" s="11" t="s">
@@ -933,7 +942,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="46"/>
       <c r="C8" s="49"/>
       <c r="D8" s="53" t="s">
@@ -949,7 +958,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <v>1</v>
       </c>
@@ -976,7 +985,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>13</v>
       </c>
@@ -996,16 +1005,16 @@
         <v>16.446124763705107</v>
       </c>
       <c r="H10" s="17">
-        <v>23.515769944341375</v>
+        <v>16.612057667103542</v>
       </c>
       <c r="I10" s="17">
-        <v>23.671497584541065</v>
+        <v>16.530120481927714</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>14</v>
       </c>
@@ -1025,16 +1034,16 @@
         <v>13.914543793768393</v>
       </c>
       <c r="H11" s="17">
-        <v>21.605794421328401</v>
+        <v>14.737727320508778</v>
       </c>
       <c r="I11" s="17">
-        <v>21.066626149054169</v>
+        <v>14.318909428896005</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>15</v>
       </c>
@@ -1054,16 +1063,16 @@
         <v>10.558107878169134</v>
       </c>
       <c r="H12" s="17">
-        <v>13.596813083132403</v>
+        <v>10.947919304465264</v>
       </c>
       <c r="I12" s="17">
-        <v>13.500425713069392</v>
+        <v>10.832159173391402</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
@@ -1083,16 +1092,16 @@
         <v>7.9507566042575029</v>
       </c>
       <c r="H13" s="17">
-        <v>8.7223291626564006</v>
+        <v>7.6972077715256395</v>
       </c>
       <c r="I13" s="17">
-        <v>8.8691064952192544</v>
+        <v>7.8120462333739908</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>9</v>
       </c>
@@ -1112,16 +1121,16 @@
         <v>11.586777369671902</v>
       </c>
       <c r="H14" s="20">
-        <v>14.835641770766502</v>
+        <v>11.619520558068045</v>
       </c>
       <c r="I14" s="20">
-        <v>14.931898109468204</v>
+        <v>11.603502944285067</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
@@ -1150,7 +1159,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -1179,7 +1188,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1217,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
         <v>16</v>
       </c>
@@ -1237,7 +1246,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1275,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
     </row>
-    <row r="20" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
         <v>13</v>
       </c>
@@ -1294,7 +1303,7 @@
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
         <v>14</v>
       </c>
@@ -1322,7 +1331,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
         <v>15</v>
       </c>
@@ -1350,7 +1359,7 @@
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
         <v>16</v>
       </c>
@@ -1378,7 +1387,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="2:12" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
         <v>9</v>
       </c>
@@ -1406,7 +1415,7 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
         <v>13</v>
       </c>
@@ -1434,7 +1443,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>14</v>
       </c>
@@ -1462,7 +1471,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
         <v>15</v>
       </c>
@@ -1490,7 +1499,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
         <v>16</v>
       </c>
@@ -1518,7 +1527,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="2:12" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="26" t="s">
         <v>9</v>
       </c>
@@ -1546,7 +1555,7 @@
       <c r="J29" s="21"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
         <v>13</v>
       </c>
@@ -1574,7 +1583,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="23" t="s">
         <v>14</v>
       </c>
@@ -1602,7 +1611,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="23" t="s">
         <v>15</v>
       </c>
@@ -1630,7 +1639,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
         <v>16</v>
       </c>
@@ -1658,7 +1667,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="26" t="s">
         <v>9</v>
       </c>
@@ -1686,7 +1695,7 @@
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
     </row>
-    <row r="35" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
         <v>13</v>
       </c>
@@ -1714,7 +1723,7 @@
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="23" t="s">
         <v>14</v>
       </c>
@@ -1742,7 +1751,7 @@
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
         <v>15</v>
       </c>
@@ -1770,7 +1779,7 @@
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="s">
         <v>16</v>
       </c>
@@ -1798,7 +1807,7 @@
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="26" t="s">
         <v>9</v>
       </c>
@@ -1826,7 +1835,7 @@
       <c r="J39" s="21"/>
       <c r="K39" s="21"/>
     </row>
-    <row r="40" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="23" t="s">
         <v>13</v>
       </c>
@@ -1854,7 +1863,7 @@
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="23" t="s">
         <v>14</v>
       </c>
@@ -1882,7 +1891,7 @@
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="23" t="s">
         <v>15</v>
       </c>
@@ -1910,7 +1919,7 @@
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="s">
         <v>16</v>
       </c>
@@ -1938,7 +1947,7 @@
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="26" t="s">
         <v>9</v>
       </c>
@@ -1966,7 +1975,7 @@
       <c r="J44" s="21"/>
       <c r="K44" s="21"/>
     </row>
-    <row r="45" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="23" t="s">
         <v>13</v>
       </c>
@@ -1994,7 +2003,7 @@
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
     </row>
-    <row r="46" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="23" t="s">
         <v>14</v>
       </c>
@@ -2022,7 +2031,7 @@
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="23" t="s">
         <v>15</v>
       </c>
@@ -2050,7 +2059,7 @@
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="23" t="s">
         <v>16</v>
       </c>
@@ -2078,7 +2087,7 @@
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="26" t="s">
         <v>9</v>
       </c>
@@ -2106,7 +2115,7 @@
       <c r="J49" s="21"/>
       <c r="K49" s="21"/>
     </row>
-    <row r="50" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="23" t="s">
         <v>13</v>
       </c>
@@ -2134,7 +2143,7 @@
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
     </row>
-    <row r="51" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="23" t="s">
         <v>14</v>
       </c>
@@ -2162,7 +2171,7 @@
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
     </row>
-    <row r="52" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="23" t="s">
         <v>15</v>
       </c>
@@ -2190,7 +2199,7 @@
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
     </row>
-    <row r="53" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
         <v>16</v>
       </c>
@@ -2218,7 +2227,7 @@
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="26" t="s">
         <v>9</v>
       </c>
@@ -2246,7 +2255,7 @@
       <c r="J54" s="21"/>
       <c r="K54" s="21"/>
     </row>
-    <row r="55" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
         <v>13</v>
       </c>
@@ -2274,7 +2283,7 @@
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
     </row>
-    <row r="56" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
         <v>14</v>
       </c>
@@ -2302,7 +2311,7 @@
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
         <v>15</v>
       </c>
@@ -2330,7 +2339,7 @@
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
         <v>16</v>
       </c>
@@ -2358,7 +2367,7 @@
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="26" t="s">
         <v>9</v>
       </c>
@@ -2386,7 +2395,7 @@
       <c r="J59" s="21"/>
       <c r="K59" s="21"/>
     </row>
-    <row r="60" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="23" t="s">
         <v>13</v>
       </c>
@@ -2414,7 +2423,7 @@
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
     </row>
-    <row r="61" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
         <v>14</v>
       </c>
@@ -2442,7 +2451,7 @@
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
     </row>
-    <row r="62" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
         <v>15</v>
       </c>
@@ -2470,7 +2479,7 @@
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
     </row>
-    <row r="63" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="23" t="s">
         <v>16</v>
       </c>
@@ -2498,7 +2507,7 @@
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
     </row>
-    <row r="64" spans="2:11" s="30" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" s="30" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="26" t="s">
         <v>9</v>
       </c>
@@ -2526,7 +2535,7 @@
       <c r="J64" s="29"/>
       <c r="K64" s="29"/>
     </row>
-    <row r="65" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="31"/>
       <c r="C65" s="31"/>
       <c r="D65" s="32"/>
@@ -2538,7 +2547,7 @@
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
     </row>
-    <row r="66" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="34"/>
       <c r="C66" s="35"/>
       <c r="D66" s="36"/>
@@ -2550,7 +2559,7 @@
       <c r="J66" s="8"/>
       <c r="K66" s="8"/>
     </row>
-    <row r="67" spans="2:11" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="43" t="s">
         <v>17</v>
       </c>
@@ -2564,7 +2573,7 @@
       <c r="J67" s="43"/>
       <c r="K67" s="8"/>
     </row>
-    <row r="68" spans="2:11" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="43" t="s">
         <v>18</v>
       </c>
@@ -2578,7 +2587,7 @@
       <c r="J68" s="43"/>
       <c r="K68" s="8"/>
     </row>
-    <row r="69" spans="2:11" s="37" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" s="37" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="38" t="s">
         <v>19</v>
       </c>
@@ -2592,7 +2601,7 @@
       <c r="J69" s="39"/>
       <c r="K69" s="8"/>
     </row>
-    <row r="70" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="40"/>
       <c r="C70" s="40"/>
       <c r="D70" s="39"/>
@@ -2603,7 +2612,7 @@
       <c r="I70" s="39"/>
       <c r="J70" s="39"/>
     </row>
-    <row r="71" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="41" t="s">
         <v>20</v>
       </c>
@@ -2616,150 +2625,150 @@
       <c r="I71" s="39"/>
       <c r="J71" s="39"/>
     </row>
-    <row r="72" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="2:11" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3">
       <c r="B75" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="2:11" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3">
       <c r="B76" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="2:11" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="2:11" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="2:11" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="2:11" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="81" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="82" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="83" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="84" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="85" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="86" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="87" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="88" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="89" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="90" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="91" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="92" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="93" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="94" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="95" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="96" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="97" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="98" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="99" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="100" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="101" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="102" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="103" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="104" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="105" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="106" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="107" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="108" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="109" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="110" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="111" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="112" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="113" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="114" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="115" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="116" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="117" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="118" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="119" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="120" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="121" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="122" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="123" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="124" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="125" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="126" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="127" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="128" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="129" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="130" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="131" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="132" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="133" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="134" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="135" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="136" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="137" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="138" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="139" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="140" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="141" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="142" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="143" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="144" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="145" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="146" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="147" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="148" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="149" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="150" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="151" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="152" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="153" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="154" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="155" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="156" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="157" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="158" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="159" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="160" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="161" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="162" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="163" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="164" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="165" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="166" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="167" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="168" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="169" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="170" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="171" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="172" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="173" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="174" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="175" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="176" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="177" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="178" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="179" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="180" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="181" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="182" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="183" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="184" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="185" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="186" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="187" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="188" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="189" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="190" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="191" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="192" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:11" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:11" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="2:11" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="81" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="82" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="83" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="84" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="85" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="86" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="87" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="88" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="89" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="90" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="91" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="92" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="93" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="94" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="95" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="96" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="97" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="98" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="99" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="100" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="101" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="102" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="103" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="104" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="105" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="106" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="107" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="108" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="109" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="110" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="111" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="112" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="113" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="114" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="115" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="116" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="117" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="118" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="119" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="120" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="121" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="122" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="123" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="124" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="125" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="126" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="127" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="128" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="129" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="130" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="131" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="132" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="133" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="134" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="135" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="136" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="137" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="138" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="139" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="140" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="141" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="142" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="143" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="144" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="145" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="146" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="147" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="148" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="149" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="150" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="151" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="152" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="153" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="154" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="155" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="156" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="157" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="158" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="159" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="160" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="161" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="162" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="163" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="164" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="165" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="166" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="167" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="168" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="169" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="170" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="171" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="172" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="173" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="174" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="175" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="176" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="177" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="178" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="179" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="180" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="181" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="182" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="183" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="184" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="185" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="186" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="187" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="188" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="189" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="190" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="191" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="192" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="193" spans="2:10" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="194" spans="2:10" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="195" spans="2:10" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="196" spans="2:10" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="197" spans="2:10" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="198" spans="2:10" s="10" customFormat="1" ht="7.8" x14ac:dyDescent="0.3"/>
+    <row r="199" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B199" s="10"/>
       <c r="C199" s="10"/>
       <c r="D199" s="10"/>
@@ -2770,7 +2779,7 @@
       <c r="I199" s="10"/>
       <c r="J199" s="10"/>
     </row>
-    <row r="200" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B200" s="10"/>
       <c r="C200" s="10"/>
       <c r="D200" s="10"/>

</xml_diff>